<commit_message>
BIR libs configuration - no predictive model
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/50_Inst_Customer_Unit.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/50_Inst_Customer_Unit.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="210" yWindow="450" windowWidth="28440" windowHeight="14235" activeTab="1"/>
+    <workbookView xWindow="210" yWindow="450" windowWidth="28440" windowHeight="14235" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_Unit" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="54">
   <si>
     <t>Customer_Unit</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>COUNTERPARTY_KOPER</t>
+  </si>
+  <si>
+    <t>BE-COUNTERPARTY_BIR</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_BIR</t>
   </si>
 </sst>
 </file>
@@ -531,6 +537,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9705975"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -742,6 +796,54 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9772650" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1183,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,6 +1390,26 @@
         <v>51</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1299,7 +1421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Static Filter Indicators updated
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/50_Inst_Customer_Unit.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/50_Inst_Customer_Unit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="210" yWindow="450" windowWidth="28440" windowHeight="14235" activeTab="2"/>
+    <workbookView xWindow="210" yWindow="450" windowWidth="28440" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_Unit" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="55">
   <si>
     <t>Customer_Unit</t>
   </si>
@@ -173,9 +173,6 @@
     <t>CUSTOMER_ANALYSIS_UNIT_BE</t>
   </si>
   <si>
-    <t>TEWSA0D</t>
-  </si>
-  <si>
     <t>COUNTERPARTY_BIB</t>
   </si>
   <si>
@@ -231,12 +228,18 @@
   </si>
   <si>
     <t>COUNTERPARTY_BIR</t>
+  </si>
+  <si>
+    <t>SEWSA0W</t>
+  </si>
+  <si>
+    <t>SEWSA0D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -585,6 +588,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9705975"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -868,6 +919,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9772650" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -947,6 +1046,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -982,6 +1098,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1160,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,10 +1351,10 @@
         <v>8</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1238,19 +1371,19 @@
         <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" t="s">
         <v>41</v>
       </c>
-      <c r="H3" t="s">
-        <v>42</v>
-      </c>
       <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" t="s">
         <v>39</v>
-      </c>
-      <c r="J3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1258,22 +1391,22 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>44</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
         <v>45</v>
-      </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1287,15 +1420,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="2" max="4" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1335,19 +1467,19 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1355,19 +1487,19 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1375,19 +1507,19 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1395,19 +1527,19 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1421,7 +1553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Configurate istanze e librerire ISPRO
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/50_Inst_Customer_Unit.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/50_Inst_Customer_Unit.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="210" yWindow="450" windowWidth="28440" windowHeight="14235" activeTab="1"/>
+    <workbookView xWindow="210" yWindow="450" windowWidth="28440" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_Unit" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="61">
   <si>
     <t>Customer_Unit</t>
   </si>
@@ -246,12 +246,18 @@
   </si>
   <si>
     <t>COUNTERPARTY_CIB</t>
+  </si>
+  <si>
+    <t>BE-COUNTERPARTY_ISPRO</t>
+  </si>
+  <si>
+    <t>COUNTERPARTY_ISPRO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -744,6 +750,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9705975"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1171,6 +1225,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9953625" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1250,6 +1352,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1285,6 +1404,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1463,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,6 +1886,26 @@
       </c>
       <c r="F8" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix  vari cib ispro isba
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/50_Inst_Customer_Unit.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/50_Inst_Customer_Unit.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alberto.collu\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="210" yWindow="450" windowWidth="28440" windowHeight="14235" activeTab="1"/>
+    <workbookView xWindow="210" yWindow="450" windowWidth="28440" windowHeight="14235" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_Unit" sheetId="1" r:id="rId1"/>
@@ -236,12 +236,6 @@
     <t>COUNTERPARTY_ALEX</t>
   </si>
   <si>
-    <t>TEWSA0D</t>
-  </si>
-  <si>
-    <t>TEWSA0W</t>
-  </si>
-  <si>
     <t>BE-COUNTERPARTY_CIB</t>
   </si>
   <si>
@@ -258,12 +252,18 @@
   </si>
   <si>
     <t>COUNTERPARTY_ISBA</t>
+  </si>
+  <si>
+    <t>EWSA0D</t>
+  </si>
+  <si>
+    <t>EWSA0W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -349,7 +349,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -392,7 +398,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="2" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -435,7 +447,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -483,7 +501,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -531,7 +555,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -579,7 +609,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -627,7 +663,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -675,7 +717,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -723,7 +771,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -771,7 +825,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -819,7 +879,67 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9705975"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -872,7 +992,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2050" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="2050" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -915,7 +1041,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="2" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -958,7 +1090,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1006,7 +1144,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1054,7 +1198,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 2"/>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1102,7 +1252,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 2"/>
+        <xdr:cNvPr id="6" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1150,7 +1306,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 2"/>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1198,7 +1360,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="AutoShape 2"/>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1246,7 +1414,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1294,7 +1468,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="AutoShape 2"/>
+        <xdr:cNvPr id="10" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1342,7 +1522,67 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="AutoShape 2"/>
+        <xdr:cNvPr id="11" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9953625" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1454,6 +1694,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1489,6 +1746,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1668,7 +1942,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,7 +2019,7 @@
         <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
         <v>40</v>
@@ -1774,7 +2048,7 @@
         <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="I4" t="s">
         <v>46</v>
@@ -1794,7 +2068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -1941,19 +2215,19 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
         <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1961,19 +2235,19 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
         <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1981,19 +2255,19 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
         <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2007,7 +2281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>